<commit_message>
VERSION 1.1.0 "C6 y Matriz Aleatoria"
</commit_message>
<xml_diff>
--- a/TOPSIS Feb2024/Experimentos/Experimentos.xlsx
+++ b/TOPSIS Feb2024/Experimentos/Experimentos.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -37,10 +37,10 @@
     <t>TOPSIS</t>
   </si>
   <si>
-    <t>09:26:41.825649</t>
-  </si>
-  <si>
-    <t>09:26:41.865294</t>
+    <t>11:51:13.715692</t>
+  </si>
+  <si>
+    <t>11:51:13.748671</t>
   </si>
   <si>
     <t>C1</t>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
   </si>
   <si>
     <t>A1</t>
@@ -485,7 +488,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="3">
-        <v>4.588541666666667E-07</v>
+        <v>3.817013888888889E-07</v>
       </c>
     </row>
   </sheetData>
@@ -495,7 +498,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -511,7 +514,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -519,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -527,7 +530,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.03</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -535,7 +538,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.07000000000000001</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -543,7 +546,15 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.3</v>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -553,13 +564,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -575,10 +586,13 @@
       <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>0.048</v>
@@ -595,10 +609,13 @@
       <c r="F2">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>0.053</v>
@@ -615,10 +632,13 @@
       <c r="F3">
         <v>0.058</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>0.057</v>
@@ -635,10 +655,13 @@
       <c r="F4">
         <v>0.022</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>0.062</v>
@@ -655,10 +678,13 @@
       <c r="F5">
         <v>0.007</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>0.066</v>
@@ -675,10 +701,13 @@
       <c r="F6">
         <v>0.004</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>0.07000000000000001</v>
@@ -695,10 +724,13 @@
       <c r="F7">
         <v>0.003</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>0.075</v>
@@ -715,10 +747,13 @@
       <c r="F8">
         <v>0.002</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>0.079</v>
@@ -735,10 +770,13 @@
       <c r="F9">
         <v>0.002</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>0.083</v>
@@ -754,6 +792,9 @@
       </c>
       <c r="F10">
         <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0.19</v>
       </c>
     </row>
   </sheetData>
@@ -779,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -787,7 +828,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>